<commit_message>
end collect data in xlsx
</commit_message>
<xml_diff>
--- a/Assignment1/result.xlsx
+++ b/Assignment1/result.xlsx
@@ -324,140 +324,166 @@
         </table:table-row>
         <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>N=256,Thread=1, Min=0, max=1000</text:p>
-          </table:table-cell>
-          <table:table-cell table:number-columns-repeated="3"/>
-        </table:table-row>
-        <table:table-row table:style-name="ro1">
-          <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>N=256,Thread=1, Min=0, max=1000</text:p>
-          </table:table-cell>
-          <table:table-cell table:number-columns-repeated="3"/>
-        </table:table-row>
-        <table:table-row table:style-name="ro1">
-          <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>N=256,Thread=1, Min=0, max=1000</text:p>
-          </table:table-cell>
-          <table:table-cell table:number-columns-repeated="3"/>
-        </table:table-row>
-        <table:table-row table:style-name="ro1">
-          <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>N=256,Thread=1, Min=0, max=1000</text:p>
-          </table:table-cell>
-          <table:table-cell table:number-columns-repeated="3"/>
-        </table:table-row>
-        <table:table-row table:style-name="ro1">
-          <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>N=256,Thread=1, Min=0, max=1000</text:p>
-          </table:table-cell>
-          <table:table-cell table:number-columns-repeated="3"/>
-        </table:table-row>
-        <table:table-row table:style-name="ro1">
-          <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>N=256,Thread=1, Min=0, max=1000</text:p>
-          </table:table-cell>
-          <table:table-cell table:number-columns-repeated="3"/>
-        </table:table-row>
-        <table:table-row table:style-name="ro1">
-          <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>N=256,Thread=1, Min=0, max=1000</text:p>
-          </table:table-cell>
-          <table:table-cell table:number-columns-repeated="3"/>
-        </table:table-row>
-        <table:table-row table:style-name="ro1">
-          <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>N=256,Thread=1, Min=0, max=1000</text:p>
-          </table:table-cell>
-          <table:table-cell table:number-columns-repeated="3"/>
-        </table:table-row>
-        <table:table-row table:style-name="ro1">
-          <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>N=256,Thread=1, Min=0, max=1000</text:p>
-          </table:table-cell>
-          <table:table-cell table:number-columns-repeated="3"/>
-        </table:table-row>
-        <table:table-row table:style-name="ro1">
-          <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>N=256,Thread=1, Min=0, max=1000</text:p>
-          </table:table-cell>
-          <table:table-cell table:number-columns-repeated="3"/>
+            <text:p>N=256,Thread=2, Min=0, max=1000</text:p>
+          </table:table-cell>
+          <table:table-cell/>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>8.84593</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>8.54937</text:p>
+          </table:table-cell>
+        </table:table-row>
+        <table:table-row table:style-name="ro1">
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>N=256,Thread=4, Min=0, max=1000</text:p>
+          </table:table-cell>
+          <table:table-cell/>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>5.23857</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>4.77091</text:p>
+          </table:table-cell>
+        </table:table-row>
+        <table:table-row table:style-name="ro1">
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>N=256,Thread=8, Min=0, max=1000</text:p>
+          </table:table-cell>
+          <table:table-cell/>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>3.54753</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>2.85949</text:p>
+          </table:table-cell>
+        </table:table-row>
+        <table:table-row table:style-name="ro1">
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>N=256,Thread=16, Min=0, max=1000</text:p>
+          </table:table-cell>
+          <table:table-cell/>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>2.67643</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>1.99214</text:p>
+          </table:table-cell>
+        </table:table-row>
+        <table:table-row table:style-name="ro1">
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>N=256,Thread=32, Min=0, max=1000</text:p>
+          </table:table-cell>
+          <table:table-cell/>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>2.21867</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>1.69124</text:p>
+          </table:table-cell>
+        </table:table-row>
+        <table:table-row table:style-name="ro1">
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>N=256,Thread=40, Min=0, max=1000</text:p>
+          </table:table-cell>
+          <table:table-cell/>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>2.23406</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>1.67213</text:p>
+          </table:table-cell>
         </table:table-row>
         <table:table-row table:style-name="ro1">
           <table:table-cell table:number-columns-repeated="4"/>
         </table:table-row>
         <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>N=512,Thread=1, Min=0, max=1000, Estim seq=0.074382</text:p>
-          </table:table-cell>
-          <table:table-cell table:number-columns-repeated="3"/>
-        </table:table-row>
-        <table:table-row table:style-name="ro1">
-          <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>N=512,Thread=1, Min=0, max=1000</text:p>
-          </table:table-cell>
-          <table:table-cell table:number-columns-repeated="3"/>
-        </table:table-row>
-        <table:table-row table:style-name="ro1">
-          <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>N=512,Thread=1, Min=0, max=1000</text:p>
-          </table:table-cell>
-          <table:table-cell table:number-columns-repeated="3"/>
-        </table:table-row>
-        <table:table-row table:style-name="ro1">
-          <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>N=512,Thread=1, Min=0, max=1000</text:p>
-          </table:table-cell>
-          <table:table-cell table:number-columns-repeated="3"/>
-        </table:table-row>
-        <table:table-row table:style-name="ro1">
-          <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>N=512,Thread=1, Min=0, max=1000</text:p>
-          </table:table-cell>
-          <table:table-cell table:number-columns-repeated="3"/>
-        </table:table-row>
-        <table:table-row table:style-name="ro1">
-          <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>N=512,Thread=1, Min=0, max=1000</text:p>
-          </table:table-cell>
-          <table:table-cell table:number-columns-repeated="3"/>
-        </table:table-row>
-        <table:table-row table:style-name="ro1">
-          <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>N=512,Thread=1, Min=0, max=1000</text:p>
-          </table:table-cell>
-          <table:table-cell table:number-columns-repeated="3"/>
-        </table:table-row>
-        <table:table-row table:style-name="ro1">
-          <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>N=512,Thread=1, Min=0, max=1000</text:p>
-          </table:table-cell>
-          <table:table-cell table:number-columns-repeated="3"/>
-        </table:table-row>
-        <table:table-row table:style-name="ro1">
-          <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>N=512,Thread=1, Min=0, max=1000</text:p>
-          </table:table-cell>
-          <table:table-cell table:number-columns-repeated="3"/>
-        </table:table-row>
-        <table:table-row table:style-name="ro1">
-          <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>N=512,Thread=1, Min=0, max=1000</text:p>
-          </table:table-cell>
-          <table:table-cell table:number-columns-repeated="3"/>
-        </table:table-row>
-        <table:table-row table:style-name="ro1">
-          <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>N=512,Thread=1, Min=0, max=1000</text:p>
-          </table:table-cell>
-          <table:table-cell table:number-columns-repeated="3"/>
-        </table:table-row>
-        <table:table-row table:style-name="ro1">
-          <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>N=512,Thread=1, Min=0, max=1000</text:p>
-          </table:table-cell>
-          <table:table-cell table:number-columns-repeated="3"/>
-        </table:table-row>
-        <table:table-row table:style-name="ro1" table:number-rows-repeated="1048527">
+            <text:p>N=512,Thread=1, Min=0, max=1000, Estim seq=65.540021</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>65.5842</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>65.5841</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>65.5833</text:p>
+          </table:table-cell>
+        </table:table-row>
+        <table:table-row table:style-name="ro1">
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>N=512,Thread=2, Min=0, max=1000</text:p>
+          </table:table-cell>
+          <table:table-cell/>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>34.2837</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>33.4536</text:p>
+          </table:table-cell>
+        </table:table-row>
+        <table:table-row table:style-name="ro1">
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>N=512,Thread=4, Min=0, max=1000</text:p>
+          </table:table-cell>
+          <table:table-cell/>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>17.5524</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>16.5471</text:p>
+          </table:table-cell>
+        </table:table-row>
+        <table:table-row table:style-name="ro1">
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>N=512,Thread=8, Min=0, max=1000</text:p>
+          </table:table-cell>
+          <table:table-cell/>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>9.32986</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>8.40291</text:p>
+          </table:table-cell>
+        </table:table-row>
+        <table:table-row table:style-name="ro1">
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>N=512,Thread=16, Min=0, max=1000</text:p>
+          </table:table-cell>
+          <table:table-cell/>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>8.36034</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>6.35851</text:p>
+          </table:table-cell>
+        </table:table-row>
+        <table:table-row table:style-name="ro1">
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>N=512,Thread=32, Min=0, max=1000</text:p>
+          </table:table-cell>
+          <table:table-cell/>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>7.24261</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>5.25371</text:p>
+          </table:table-cell>
+        </table:table-row>
+        <table:table-row table:style-name="ro1">
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>N=512,Thread=40, Min=0, max=1000</text:p>
+          </table:table-cell>
+          <table:table-cell/>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>7.19698</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>5.20369</text:p>
+          </table:table-cell>
+        </table:table-row>
+        <table:table-row table:style-name="ro1" table:number-rows-repeated="1048536">
           <table:table-cell table:number-columns-repeated="4"/>
         </table:table-row>
         <table:table-row table:style-name="ro1">
@@ -474,11 +500,11 @@
 <office:document-meta xmlns:grddl="http://www.w3.org/2003/g/data-view#" xmlns:meta="urn:oasis:names:tc:opendocument:xmlns:meta:1.0" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:xlink="http://www.w3.org/1999/xlink" xmlns:ooo="http://openoffice.org/2004/office" xmlns:office="urn:oasis:names:tc:opendocument:xmlns:office:1.0" office:version="1.3">
   <office:meta>
     <meta:creation-date>2024-04-09T17:52:10.097789529</meta:creation-date>
-    <dc:date>2024-04-11T18:49:15.991208518</dc:date>
-    <meta:editing-duration>PT1H47M9S</meta:editing-duration>
-    <meta:editing-cycles>14</meta:editing-cycles>
+    <dc:date>2024-04-12T10:42:06.784172451</dc:date>
+    <meta:editing-duration>PT3H26M40S</meta:editing-duration>
+    <meta:editing-cycles>17</meta:editing-cycles>
     <meta:generator>LibreOffice/7.6.6.3$Linux_X86_64 LibreOffice_project/60$Build-3</meta:generator>
-    <meta:document-statistic meta:table-count="1" meta:cell-count="90" meta:object-count="0"/>
+    <meta:document-statistic meta:table-count="1" meta:cell-count="108" meta:object-count="0"/>
   </office:meta>
 </office:document-meta>
 </file>
@@ -490,19 +516,19 @@
       <config:config-item config:name="VisibleAreaTop" config:type="int">0</config:config-item>
       <config:config-item config:name="VisibleAreaLeft" config:type="int">0</config:config-item>
       <config:config-item config:name="VisibleAreaWidth" config:type="int">16686</config:config-item>
-      <config:config-item config:name="VisibleAreaHeight" config:type="int">21675</config:config-item>
+      <config:config-item config:name="VisibleAreaHeight" config:type="int">17611</config:config-item>
       <config:config-item-map-indexed config:name="Views">
         <config:config-item-map-entry>
           <config:config-item config:name="ViewId" config:type="string">view1</config:config-item>
           <config:config-item-map-named config:name="Tables">
             <config:config-item-map-entry config:name="Sheet1">
-              <config:config-item config:name="CursorPositionX" config:type="int">2</config:config-item>
-              <config:config-item config:name="CursorPositionY" config:type="int">29</config:config-item>
+              <config:config-item config:name="CursorPositionX" config:type="int">3</config:config-item>
+              <config:config-item config:name="CursorPositionY" config:type="int">34</config:config-item>
               <config:config-item config:name="ActiveSplitRange" config:type="short">2</config:config-item>
               <config:config-item config:name="PositionLeft" config:type="int">0</config:config-item>
               <config:config-item config:name="PositionRight" config:type="int">0</config:config-item>
               <config:config-item config:name="PositionTop" config:type="int">0</config:config-item>
-              <config:config-item config:name="PositionBottom" config:type="int">3</config:config-item>
+              <config:config-item config:name="PositionBottom" config:type="int">0</config:config-item>
               <config:config-item config:name="ZoomType" config:type="short">0</config:config-item>
               <config:config-item config:name="ZoomValue" config:type="int">100</config:config-item>
               <config:config-item config:name="PageViewZoomValue" config:type="int">60</config:config-item>
@@ -575,7 +601,7 @@
       <config:config-item config:name="LoadReadonly" config:type="boolean">false</config:config-item>
       <config:config-item config:name="PrinterName" config:type="string">Generic Printer</config:config-item>
       <config:config-item config:name="PrinterPaperFromSetup" config:type="boolean">false</config:config-item>
-      <config:config-item config:name="PrinterSetup" config:type="base64Binary">1gH+/0dlbmVyaWMgUHJpbnRlcgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAU0dFTlBSVAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAWAAMAwgAAAAAAAAAEAAhSAAAEdAAASm9iRGF0YSAxCnByaW50ZXI9R2VuZXJpYyBQcmludGVyCm9yaWVudGF0aW9uPVBvcnRyYWl0CmNvcGllcz0xCmNvbGxhdGU9ZmFsc2UKbWFyZ2luYWRqdXN0bWVudD0wLDAsJzAsMApjb2xvcmRlcHRoPTI0CnBzbGV2ZWw9MApwZGZkZXZpY2U9MQpjb2xvcmRldmljZT0wClBQRENvbnRleHREYXRhCkR1cGxleDpOb25lAFBhZ2VTaXplOkE0AAASAENPTVBBVF9EVVBMRVhfTU9ERQ8ARHVwbGV4TW9kZTo6T2ZmDABQUklOVEVSX05BTUUPAEdlbmVyaWMgUHJpbnRlcgsARFJJVkVSX05BTUUHAFNHRU5QUlQ=</config:config-item>
+      <config:config-item config:name="PrinterSetup" config:type="base64Binary">1gH+/0dlbmVyaWMgUHJpbnRlcgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAU0dFTlBSVAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAWAAMAwgAAAAAAAAAEAAhSAAAEdAAASm9iRGF0YSAxCnByaW50ZXI9R2VuZXJpYyBQcmludGVyCm9yaWVudGF0aW9uPVBvcnRyYWl0CmNvcGllcz0xCmNvbGxhdGU9ZmFsc2UKbWFyZ2luYWRqdXN0bWVudD0wLDAsJzAsMApjb2xvcmRlcHRoPTI0CnBzbGV2ZWw9MApwZGZkZXZpY2U9MQpjb2xvcmRldmljZT0wClBQRENvbnRleHREYXRhClBhZ2VTaXplOkE0AER1cGxleDpOb25lAAASAENPTVBBVF9EVVBMRVhfTU9ERQ8ARHVwbGV4TW9kZTo6T2ZmDABQUklOVEVSX05BTUUPAEdlbmVyaWMgUHJpbnRlcgsARFJJVkVSX05BTUUHAFNHRU5QUlQ=</config:config-item>
       <config:config-item config:name="RasterIsVisible" config:type="boolean">false</config:config-item>
       <config:config-item config:name="RasterResolutionX" config:type="int">1000</config:config-item>
       <config:config-item config:name="RasterResolutionY" config:type="int">1000</config:config-item>
@@ -757,9 +783,9 @@
         </style:region-left>
         <style:region-right>
           <text:p>
-            <text:date style:data-style-name="N2" text:date-value="2024-04-11">00/00/0000</text:date>
+            <text:date style:data-style-name="N2" text:date-value="2024-04-12">00/00/0000</text:date>
             , 
-            <text:time style:data-style-name="N2" text:time-value="18:03:48.753167352">00:00:00</text:time>
+            <text:time style:data-style-name="N2" text:time-value="09:02:35.425497321">00:00:00</text:time>
           </text:p>
         </style:region-right>
       </style:header>

</xml_diff>

<commit_message>
fix value and add omp version
</commit_message>
<xml_diff>
--- a/Assignment1/result.xlsx
+++ b/Assignment1/result.xlsx
@@ -104,14 +104,14 @@
             <text:p>N=4,Thread=2, Min=0, max=1000</text:p>
           </table:table-cell>
           <table:table-cell/>
-          <table:table-cell table:style-name="ce2" office:value-type="float" office:value="0.00356625" calcext:value-type="float">
-            <text:p>0,00356625</text:p>
+          <table:table-cell table:style-name="ce2" office:value-type="float" office:value="0.00324217" calcext:value-type="float">
+            <text:p>0,00324217</text:p>
           </table:table-cell>
           <table:table-cell table:style-name="ce6" office:value-type="float" office:value="0.00313312" calcext:value-type="float">
             <text:p>0,00313312</text:p>
           </table:table-cell>
-          <table:table-cell table:formula="of:=[.B2]/[.C3]" office:value-type="float" office:value="1.14665825446898" calcext:value-type="float">
-            <text:p>1,14665825446898</text:p>
+          <table:table-cell table:formula="of:=[.B2]/[.C3]" office:value-type="float" office:value="1.26127562712628" calcext:value-type="float">
+            <text:p>1,26127562712628</text:p>
           </table:table-cell>
           <table:table-cell table:formula="of:=[.B2]/[.D3]" office:value-type="float" office:value="1.30517503319375" calcext:value-type="float">
             <text:p>1,30517503319375</text:p>
@@ -122,14 +122,14 @@
             <text:p>N=4,Thread=4, Min=0, max=1000</text:p>
           </table:table-cell>
           <table:table-cell/>
-          <table:table-cell table:style-name="ce2" office:value-type="float" office:value="0.00331601" calcext:value-type="float">
-            <text:p>0,00331601</text:p>
+          <table:table-cell table:style-name="ce2" office:value-type="float" office:value="0.00296711" calcext:value-type="float">
+            <text:p>0,00296711</text:p>
           </table:table-cell>
           <table:table-cell table:style-name="ce6" office:value-type="float" office:value="0.00295609" calcext:value-type="float">
             <text:p>0,00295609</text:p>
           </table:table-cell>
-          <table:table-cell table:formula="of:=[.B2]/[.C4]" office:value-type="float" office:value="1.23318988784714" calcext:value-type="float">
-            <text:p>1,23318988784714</text:p>
+          <table:table-cell table:formula="of:=[.B2]/[.C4]" office:value-type="float" office:value="1.37819966229766" calcext:value-type="float">
+            <text:p>1,37819966229766</text:p>
           </table:table-cell>
           <table:table-cell table:formula="of:=[.B2]/[.D4]" office:value-type="float" office:value="1.38333744913044" calcext:value-type="float">
             <text:p>1,38333744913044</text:p>
@@ -163,14 +163,14 @@
             <text:p>N=8,Thread=2, Min=0, max=1000</text:p>
           </table:table-cell>
           <table:table-cell/>
-          <table:table-cell office:value-type="float" office:value="0.0130884" calcext:value-type="float">
-            <text:p>0,0130884</text:p>
+          <table:table-cell office:value-type="float" office:value="0.0128219" calcext:value-type="float">
+            <text:p>0,0128219</text:p>
           </table:table-cell>
           <table:table-cell office:value-type="float" office:value="0.0124747" calcext:value-type="float">
             <text:p>0,0124747</text:p>
           </table:table-cell>
-          <table:table-cell table:formula="of:=[.B6]/[.C7]" office:value-type="float" office:value="1.58103358699306" calcext:value-type="float">
-            <text:p>1,58103358699306</text:p>
+          <table:table-cell table:formula="of:=[.B6]/[.C7]" office:value-type="float" office:value="1.61389497656354" calcext:value-type="float">
+            <text:p>1,61389497656354</text:p>
           </table:table-cell>
           <table:table-cell table:formula="of:=[.B6]/[.D7]" office:value-type="float" office:value="1.65881343839932" calcext:value-type="float">
             <text:p>1,65881343839932</text:p>
@@ -181,14 +181,14 @@
             <text:p>N=8,Thread=4, Min=0, max=1000</text:p>
           </table:table-cell>
           <table:table-cell/>
-          <table:table-cell office:value-type="float" office:value="0.00955151" calcext:value-type="float">
-            <text:p>0,00955151</text:p>
+          <table:table-cell office:value-type="float" office:value="0.00924847" calcext:value-type="float">
+            <text:p>0,00924847</text:p>
           </table:table-cell>
           <table:table-cell office:value-type="float" office:value="0.00836691" calcext:value-type="float">
             <text:p>0,00836691</text:p>
           </table:table-cell>
-          <table:table-cell table:formula="of:=[.B6]/[.C8]" office:value-type="float" office:value="2.16648467101013" calcext:value-type="float">
-            <text:p>2,16648467101013</text:p>
+          <table:table-cell table:formula="of:=[.B6]/[.C8]" office:value-type="float" office:value="2.23747279279708" calcext:value-type="float">
+            <text:p>2,23747279279708</text:p>
           </table:table-cell>
           <table:table-cell table:formula="of:=[.B6]/[.D8]" office:value-type="float" office:value="2.4732189063824" calcext:value-type="float">
             <text:p>2,4732189063824</text:p>
@@ -199,14 +199,14 @@
             <text:p>N=8,Thread=8, Min=0, max=1000</text:p>
           </table:table-cell>
           <table:table-cell/>
-          <table:table-cell office:value-type="float" office:value="0.00778859" calcext:value-type="float">
-            <text:p>0,00778859</text:p>
+          <table:table-cell office:value-type="float" office:value="0.00746941" calcext:value-type="float">
+            <text:p>0,00746941</text:p>
           </table:table-cell>
           <table:table-cell office:value-type="float" office:value="0.00752128" calcext:value-type="float">
             <text:p>0,00752128</text:p>
           </table:table-cell>
-          <table:table-cell table:formula="of:=[.B6]/[.C9]" office:value-type="float" office:value="2.65686086955405" calcext:value-type="float">
-            <text:p>2,65686086955405</text:p>
+          <table:table-cell table:formula="of:=[.B6]/[.C9]" office:value-type="float" office:value="2.77039284227268" calcext:value-type="float">
+            <text:p>2,77039284227268</text:p>
           </table:table-cell>
           <table:table-cell table:formula="of:=[.B6]/[.D9]" office:value-type="float" office:value="2.75128701497617" calcext:value-type="float">
             <text:p>2,75128701497617</text:p>
@@ -466,17 +466,17 @@
             <text:p>N=256,Thread=2, Min=0, max=1000</text:p>
           </table:table-cell>
           <table:table-cell/>
-          <table:table-cell office:value-type="float" office:value="8.84593" calcext:value-type="float">
-            <text:p>8,84593</text:p>
-          </table:table-cell>
-          <table:table-cell office:value-type="float" office:value="8.54937" calcext:value-type="float">
-            <text:p>8,54937</text:p>
-          </table:table-cell>
-          <table:table-cell table:formula="of:=[.B25]/[.C26]" office:value-type="float" office:value="1.86421325965727" calcext:value-type="float">
-            <text:p>1,86421325965727</text:p>
-          </table:table-cell>
-          <table:table-cell table:formula="of:=[.B25]/[.D26]" office:value-type="float" office:value="1.92887897002937" calcext:value-type="float">
-            <text:p>1,92887897002937</text:p>
+          <table:table-cell office:value-type="float" office:value="8.5305" calcext:value-type="float">
+            <text:p>8,5305</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="float" office:value="8.28782" calcext:value-type="float">
+            <text:p>8,28782</text:p>
+          </table:table-cell>
+          <table:table-cell table:formula="of:=[.B25]/[.C26]" office:value-type="float" office:value="1.9331457710568" calcext:value-type="float">
+            <text:p>1,9331457710568</text:p>
+          </table:table-cell>
+          <table:table-cell table:formula="of:=[.B25]/[.D26]" office:value-type="float" office:value="1.98975122529206" calcext:value-type="float">
+            <text:p>1,98975122529206</text:p>
           </table:table-cell>
         </table:table-row>
         <table:table-row table:style-name="ro1">
@@ -484,17 +484,17 @@
             <text:p>N=256,Thread=4, Min=0, max=1000</text:p>
           </table:table-cell>
           <table:table-cell/>
-          <table:table-cell office:value-type="float" office:value="5.23857" calcext:value-type="float">
-            <text:p>5,23857</text:p>
-          </table:table-cell>
-          <table:table-cell office:value-type="float" office:value="4.77091" calcext:value-type="float">
-            <text:p>4,77091</text:p>
-          </table:table-cell>
-          <table:table-cell table:formula="of:=[.B25]/[.C27]" office:value-type="float" office:value="3.14793922769" calcext:value-type="float">
-            <text:p>3,14793922769</text:p>
-          </table:table-cell>
-          <table:table-cell table:formula="of:=[.B25]/[.D27]" office:value-type="float" office:value="3.45651039319543" calcext:value-type="float">
-            <text:p>3,45651039319543</text:p>
+          <table:table-cell office:value-type="float" office:value="4.50842" calcext:value-type="float">
+            <text:p>4,50842</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="float" office:value="4.20051" calcext:value-type="float">
+            <text:p>4,20051</text:p>
+          </table:table-cell>
+          <table:table-cell table:formula="of:=[.B25]/[.C27]" office:value-type="float" office:value="3.65775593223347" calcext:value-type="float">
+            <text:p>3,65775593223347</text:p>
+          </table:table-cell>
+          <table:table-cell table:formula="of:=[.B25]/[.D27]" office:value-type="float" office:value="3.92588042880507" calcext:value-type="float">
+            <text:p>3,92588042880507</text:p>
           </table:table-cell>
         </table:table-row>
         <table:table-row table:style-name="ro1">
@@ -502,17 +502,17 @@
             <text:p>N=256,Thread=8, Min=0, max=1000</text:p>
           </table:table-cell>
           <table:table-cell/>
-          <table:table-cell office:value-type="float" office:value="3.54753" calcext:value-type="float">
-            <text:p>3,54753</text:p>
-          </table:table-cell>
-          <table:table-cell office:value-type="float" office:value="2.85949" calcext:value-type="float">
-            <text:p>2,85949</text:p>
-          </table:table-cell>
-          <table:table-cell table:formula="of:=[.B25]/[.C28]" office:value-type="float" office:value="4.64850191541721" calcext:value-type="float">
-            <text:p>4,64850191541721</text:p>
-          </table:table-cell>
-          <table:table-cell table:formula="of:=[.B25]/[.D28]" office:value-type="float" office:value="5.76700740341809" calcext:value-type="float">
-            <text:p>5,76700740341809</text:p>
+          <table:table-cell office:value-type="float" office:value="2.45088" calcext:value-type="float">
+            <text:p>2,45088</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="float" office:value="2.16657" calcext:value-type="float">
+            <text:p>2,16657</text:p>
+          </table:table-cell>
+          <table:table-cell table:formula="of:=[.B25]/[.C28]" office:value-type="float" office:value="6.72848119858989" calcext:value-type="float">
+            <text:p>6,72848119858989</text:p>
+          </table:table-cell>
+          <table:table-cell table:formula="of:=[.B25]/[.D28]" office:value-type="float" office:value="7.61143189465376" calcext:value-type="float">
+            <text:p>7,61143189465376</text:p>
           </table:table-cell>
         </table:table-row>
         <table:table-row table:style-name="ro1">
@@ -520,17 +520,17 @@
             <text:p>N=256,Thread=16, Min=0, max=1000</text:p>
           </table:table-cell>
           <table:table-cell/>
-          <table:table-cell office:value-type="float" office:value="2.67643" calcext:value-type="float">
-            <text:p>2,67643</text:p>
-          </table:table-cell>
-          <table:table-cell office:value-type="float" office:value="1.99214" calcext:value-type="float">
-            <text:p>1,99214</text:p>
-          </table:table-cell>
-          <table:table-cell table:formula="of:=[.B25]/[.C29]" office:value-type="float" office:value="6.16145387699286" calcext:value-type="float">
-            <text:p>6,16145387699286</text:p>
-          </table:table-cell>
-          <table:table-cell table:formula="of:=[.B25]/[.D29]" office:value-type="float" office:value="8.27788207656088" calcext:value-type="float">
-            <text:p>8,27788207656088</text:p>
+          <table:table-cell office:value-type="float" office:value="1.38306" calcext:value-type="float">
+            <text:p>1,38306</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="float" office:value="1.15542" calcext:value-type="float">
+            <text:p>1,15542</text:p>
+          </table:table-cell>
+          <table:table-cell table:formula="of:=[.B25]/[.C29]" office:value-type="float" office:value="11.923343889636" calcext:value-type="float">
+            <text:p>11,923343889636</text:p>
+          </table:table-cell>
+          <table:table-cell table:formula="of:=[.B25]/[.D29]" office:value-type="float" office:value="14.2724723477177" calcext:value-type="float">
+            <text:p>14,2724723477177</text:p>
           </table:table-cell>
         </table:table-row>
         <table:table-row table:style-name="ro1">
@@ -538,17 +538,17 @@
             <text:p>N=256,Thread=32, Min=0, max=1000</text:p>
           </table:table-cell>
           <table:table-cell/>
-          <table:table-cell office:value-type="float" office:value="2.21867" calcext:value-type="float">
-            <text:p>2,21867</text:p>
-          </table:table-cell>
-          <table:table-cell office:value-type="float" office:value="1.69124" calcext:value-type="float">
-            <text:p>1,69124</text:p>
-          </table:table-cell>
-          <table:table-cell table:formula="of:=[.B25]/[.C30]" office:value-type="float" office:value="7.43269616481947" calcext:value-type="float">
-            <text:p>7,43269616481947</text:p>
-          </table:table-cell>
-          <table:table-cell table:formula="of:=[.B25]/[.D30]" office:value-type="float" office:value="9.75065632317116" calcext:value-type="float">
-            <text:p>9,75065632317116</text:p>
+          <table:table-cell office:value-type="float" office:value="0.829177" calcext:value-type="float">
+            <text:p>0,829177</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="float" office:value="0.655441" calcext:value-type="float">
+            <text:p>0,655441</text:p>
+          </table:table-cell>
+          <table:table-cell table:formula="of:=[.B25]/[.C30]" office:value-type="float" office:value="19.8880335561647" calcext:value-type="float">
+            <text:p>19,8880335561647</text:p>
+          </table:table-cell>
+          <table:table-cell table:formula="of:=[.B25]/[.D30]" office:value-type="float" office:value="25.1597016359977" calcext:value-type="float">
+            <text:p>25,1597016359977</text:p>
           </table:table-cell>
         </table:table-row>
         <table:table-row table:style-name="ro1">
@@ -556,17 +556,17 @@
             <text:p>N=256,Thread=40, Min=0, max=1000</text:p>
           </table:table-cell>
           <table:table-cell/>
-          <table:table-cell office:value-type="float" office:value="2.23406" calcext:value-type="float">
-            <text:p>2,23406</text:p>
-          </table:table-cell>
-          <table:table-cell office:value-type="float" office:value="1.67213" calcext:value-type="float">
-            <text:p>1,67213</text:p>
-          </table:table-cell>
-          <table:table-cell table:formula="of:=[.B25]/[.C31]" office:value-type="float" office:value="7.38149378261998" calcext:value-type="float">
-            <text:p>7,38149378261998</text:p>
-          </table:table-cell>
-          <table:table-cell table:formula="of:=[.B25]/[.D31]" office:value-type="float" office:value="9.86209206222004" calcext:value-type="float">
-            <text:p>9,86209206222004</text:p>
+          <table:table-cell office:value-type="float" office:value="0.716863" calcext:value-type="float">
+            <text:p>0,716863</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="float" office:value="0.558642" calcext:value-type="float">
+            <text:p>0,558642</text:p>
+          </table:table-cell>
+          <table:table-cell table:formula="of:=[.B25]/[.C31]" office:value-type="float" office:value="23.0039770500082" calcext:value-type="float">
+            <text:p>23,0039770500082</text:p>
+          </table:table-cell>
+          <table:table-cell table:formula="of:=[.B25]/[.D31]" office:value-type="float" office:value="29.519262783679" calcext:value-type="float">
+            <text:p>29,519262783679</text:p>
           </table:table-cell>
         </table:table-row>
         <table:table-row table:style-name="ro1">
@@ -597,17 +597,17 @@
             <text:p>N=512,Thread=2, Min=0, max=1000</text:p>
           </table:table-cell>
           <table:table-cell/>
-          <table:table-cell office:value-type="float" office:value="34.2837" calcext:value-type="float">
-            <text:p>34,2837</text:p>
-          </table:table-cell>
-          <table:table-cell office:value-type="float" office:value="33.4536" calcext:value-type="float">
-            <text:p>33,4536</text:p>
-          </table:table-cell>
-          <table:table-cell table:formula="of:=[.B33]/[.C34]" office:value-type="float" office:value="1.91298488786216" calcext:value-type="float">
-            <text:p>1,91298488786216</text:p>
-          </table:table-cell>
-          <table:table-cell table:formula="of:=[.B33]/[.D34]" office:value-type="float" office:value="1.96045268670636" calcext:value-type="float">
-            <text:p>1,96045268670636</text:p>
+          <table:table-cell office:value-type="float" office:value="33.6132" calcext:value-type="float">
+            <text:p>33,6132</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="float" office:value="32.868" calcext:value-type="float">
+            <text:p>32,868</text:p>
+          </table:table-cell>
+          <table:table-cell table:formula="of:=[.B33]/[.C34]" office:value-type="float" office:value="1.95114419335261" calcext:value-type="float">
+            <text:p>1,95114419335261</text:p>
+          </table:table-cell>
+          <table:table-cell table:formula="of:=[.B33]/[.D34]" office:value-type="float" office:value="1.99538152610442" calcext:value-type="float">
+            <text:p>1,99538152610442</text:p>
           </table:table-cell>
         </table:table-row>
         <table:table-row table:style-name="ro1">
@@ -651,17 +651,17 @@
             <text:p>N=512,Thread=16, Min=0, max=1000</text:p>
           </table:table-cell>
           <table:table-cell/>
-          <table:table-cell office:value-type="float" office:value="8.36034" calcext:value-type="float">
-            <text:p>8,36034</text:p>
-          </table:table-cell>
-          <table:table-cell office:value-type="float" office:value="6.35851" calcext:value-type="float">
-            <text:p>6,35851</text:p>
-          </table:table-cell>
-          <table:table-cell table:formula="of:=[.B33]/[.C37]" office:value-type="float" office:value="7.84468095795147" calcext:value-type="float">
-            <text:p>7,84468095795147</text:p>
-          </table:table-cell>
-          <table:table-cell table:formula="of:=[.B33]/[.D37]" office:value-type="float" office:value="10.3143975554021" calcext:value-type="float">
-            <text:p>10,3143975554021</text:p>
+          <table:table-cell office:value-type="float" office:value="5.09843" calcext:value-type="float">
+            <text:p>5,09843</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="float" office:value="4.34469" calcext:value-type="float">
+            <text:p>4,34469</text:p>
+          </table:table-cell>
+          <table:table-cell table:formula="of:=[.B33]/[.C37]" office:value-type="float" office:value="12.8636070319687" calcext:value-type="float">
+            <text:p>12,8636070319687</text:p>
+          </table:table-cell>
+          <table:table-cell table:formula="of:=[.B33]/[.D37]" office:value-type="float" office:value="15.0952542068594" calcext:value-type="float">
+            <text:p>15,0952542068594</text:p>
           </table:table-cell>
         </table:table-row>
         <table:table-row table:style-name="ro1">
@@ -669,17 +669,17 @@
             <text:p>N=512,Thread=32, Min=0, max=1000</text:p>
           </table:table-cell>
           <table:table-cell/>
-          <table:table-cell office:value-type="float" office:value="7.24261" calcext:value-type="float">
-            <text:p>7,24261</text:p>
-          </table:table-cell>
-          <table:table-cell office:value-type="float" office:value="5.25371" calcext:value-type="float">
-            <text:p>5,25371</text:p>
-          </table:table-cell>
-          <table:table-cell table:formula="of:=[.B33]/[.C38]" office:value-type="float" office:value="9.05532673994596" calcext:value-type="float">
-            <text:p>9,05532673994596</text:p>
-          </table:table-cell>
-          <table:table-cell table:formula="of:=[.B33]/[.D38]" office:value-type="float" office:value="12.4834069638408" calcext:value-type="float">
-            <text:p>12,4834069638408</text:p>
+          <table:table-cell office:value-type="float" office:value="2.9225" calcext:value-type="float">
+            <text:p>2,9225</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="float" office:value="2.32933" calcext:value-type="float">
+            <text:p>2,32933</text:p>
+          </table:table-cell>
+          <table:table-cell table:formula="of:=[.B33]/[.C38]" office:value-type="float" office:value="22.441129170231" calcext:value-type="float">
+            <text:p>22,441129170231</text:p>
+          </table:table-cell>
+          <table:table-cell table:formula="of:=[.B33]/[.D38]" office:value-type="float" office:value="28.1558216311128" calcext:value-type="float">
+            <text:p>28,1558216311128</text:p>
           </table:table-cell>
         </table:table-row>
         <table:table-row table:style-name="ro1">
@@ -687,17 +687,17 @@
             <text:p>N=512,Thread=40, Min=0, max=1000</text:p>
           </table:table-cell>
           <table:table-cell/>
-          <table:table-cell office:value-type="float" office:value="7.19698" calcext:value-type="float">
-            <text:p>7,19698</text:p>
-          </table:table-cell>
-          <table:table-cell office:value-type="float" office:value="5.20369" calcext:value-type="float">
-            <text:p>5,20369</text:p>
-          </table:table-cell>
-          <table:table-cell table:formula="of:=[.B33]/[.C39]" office:value-type="float" office:value="9.11273895439476" calcext:value-type="float">
-            <text:p>9,11273895439476</text:p>
-          </table:table-cell>
-          <table:table-cell table:formula="of:=[.B33]/[.D39]" office:value-type="float" office:value="12.603402585473" calcext:value-type="float">
-            <text:p>12,603402585473</text:p>
+          <table:table-cell office:value-type="float" office:value="2.46665" calcext:value-type="float">
+            <text:p>2,46665</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="float" office:value="1.92884" calcext:value-type="float">
+            <text:p>1,92884</text:p>
+          </table:table-cell>
+          <table:table-cell table:formula="of:=[.B33]/[.C39]" office:value-type="float" office:value="26.58836884033" calcext:value-type="float">
+            <text:p>26,58836884033</text:p>
+          </table:table-cell>
+          <table:table-cell table:formula="of:=[.B33]/[.D39]" office:value-type="float" office:value="34.001887144605" calcext:value-type="float">
+            <text:p>34,001887144605</text:p>
           </table:table-cell>
         </table:table-row>
         <table:table-row table:style-name="ro1" table:number-rows-repeated="1048536">
@@ -717,9 +717,9 @@
 <office:document-meta xmlns:grddl="http://www.w3.org/2003/g/data-view#" xmlns:meta="urn:oasis:names:tc:opendocument:xmlns:meta:1.0" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:xlink="http://www.w3.org/1999/xlink" xmlns:ooo="http://openoffice.org/2004/office" xmlns:office="urn:oasis:names:tc:opendocument:xmlns:office:1.0" office:version="1.3">
   <office:meta>
     <meta:creation-date>2024-04-09T17:52:10.097789529</meta:creation-date>
-    <dc:date>2024-04-14T16:33:56.546261232</dc:date>
-    <meta:editing-duration>PT4H17M7S</meta:editing-duration>
-    <meta:editing-cycles>21</meta:editing-cycles>
+    <dc:date>2024-04-14T18:21:54.437455258</dc:date>
+    <meta:editing-duration>PT5H24M5S</meta:editing-duration>
+    <meta:editing-cycles>25</meta:editing-cycles>
     <meta:generator>LibreOffice/7.6.6.3$Linux_X86_64 LibreOffice_project/60$Build-3</meta:generator>
     <meta:document-statistic meta:table-count="1" meta:cell-count="176" meta:object-count="0"/>
   </office:meta>
@@ -739,8 +739,8 @@
           <config:config-item config:name="ViewId" config:type="string">view1</config:config-item>
           <config:config-item-map-named config:name="Tables">
             <config:config-item-map-entry config:name="Sheet1">
-              <config:config-item config:name="CursorPositionX" config:type="int">5</config:config-item>
-              <config:config-item config:name="CursorPositionY" config:type="int">39</config:config-item>
+              <config:config-item config:name="CursorPositionX" config:type="int">3</config:config-item>
+              <config:config-item config:name="CursorPositionY" config:type="int">26</config:config-item>
               <config:config-item config:name="ActiveSplitRange" config:type="short">2</config:config-item>
               <config:config-item config:name="PositionLeft" config:type="int">0</config:config-item>
               <config:config-item config:name="PositionRight" config:type="int">0</config:config-item>
@@ -757,7 +757,7 @@
             </config:config-item-map-entry>
           </config:config-item-map-named>
           <config:config-item config:name="ActiveTable" config:type="string">Sheet1</config:config-item>
-          <config:config-item config:name="HorizontalScrollbarWidth" config:type="int">1847</config:config-item>
+          <config:config-item config:name="HorizontalScrollbarWidth" config:type="int">887</config:config-item>
           <config:config-item config:name="ZoomType" config:type="short">0</config:config-item>
           <config:config-item config:name="ZoomValue" config:type="int">100</config:config-item>
           <config:config-item config:name="PageViewZoomValue" config:type="int">60</config:config-item>
@@ -818,7 +818,7 @@
       <config:config-item config:name="LoadReadonly" config:type="boolean">false</config:config-item>
       <config:config-item config:name="PrinterName" config:type="string">Generic Printer</config:config-item>
       <config:config-item config:name="PrinterPaperFromSetup" config:type="boolean">false</config:config-item>
-      <config:config-item config:name="PrinterSetup" config:type="base64Binary">1gH+/0dlbmVyaWMgUHJpbnRlcgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAU0dFTlBSVAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAWAAMAwgAAAAAAAAAEAAhSAAAEdAAASm9iRGF0YSAxCnByaW50ZXI9R2VuZXJpYyBQcmludGVyCm9yaWVudGF0aW9uPVBvcnRyYWl0CmNvcGllcz0xCmNvbGxhdGU9ZmFsc2UKbWFyZ2luYWRqdXN0bWVudD0wLDAsJzAsMApjb2xvcmRlcHRoPTI0CnBzbGV2ZWw9MApwZGZkZXZpY2U9MQpjb2xvcmRldmljZT0wClBQRENvbnRleHREYXRhClBhZ2VTaXplOkE0AER1cGxleDpOb25lAAASAENPTVBBVF9EVVBMRVhfTU9ERQ8ARHVwbGV4TW9kZTo6T2ZmDABQUklOVEVSX05BTUUPAEdlbmVyaWMgUHJpbnRlcgsARFJJVkVSX05BTUUHAFNHRU5QUlQ=</config:config-item>
+      <config:config-item config:name="PrinterSetup" config:type="base64Binary">1gH+/0dlbmVyaWMgUHJpbnRlcgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAU0dFTlBSVAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAWAAMAwgAAAAAAAAAEAAhSAAAEdAAASm9iRGF0YSAxCnByaW50ZXI9R2VuZXJpYyBQcmludGVyCm9yaWVudGF0aW9uPVBvcnRyYWl0CmNvcGllcz0xCmNvbGxhdGU9ZmFsc2UKbWFyZ2luYWRqdXN0bWVudD0wLDAsJzAsMApjb2xvcmRlcHRoPTI0CnBzbGV2ZWw9MApwZGZkZXZpY2U9MQpjb2xvcmRldmljZT0wClBQRENvbnRleHREYXRhCkR1cGxleDpOb25lAFBhZ2VTaXplOkE0AAASAENPTVBBVF9EVVBMRVhfTU9ERQ8ARHVwbGV4TW9kZTo6T2ZmDABQUklOVEVSX05BTUUPAEdlbmVyaWMgUHJpbnRlcgsARFJJVkVSX05BTUUHAFNHRU5QUlQ=</config:config-item>
       <config:config-item config:name="RasterIsVisible" config:type="boolean">false</config:config-item>
       <config:config-item config:name="RasterResolutionX" config:type="int">1000</config:config-item>
       <config:config-item config:name="RasterResolutionY" config:type="int">1000</config:config-item>
@@ -1002,7 +1002,7 @@
           <text:p>
             <text:date style:data-style-name="N2" text:date-value="2024-04-14">00/00/0000</text:date>
             , 
-            <text:time style:data-style-name="N2" text:time-value="16:19:14.574673929">00:00:00</text:time>
+            <text:time style:data-style-name="N2" text:time-value="17:14:54.043208273">00:00:00</text:time>
           </text:p>
         </style:region-right>
       </style:header>

</xml_diff>